<commit_message>
added new DIC values
</commit_message>
<xml_diff>
--- a/USA/state/data/model_report/t2m_mean_1982_2013_DIC_values.xlsx
+++ b/USA/state/data/model_report/t2m_mean_1982_2013_DIC_values.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="-23080" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
   <si>
     <t>sex</t>
   </si>
@@ -50,10 +50,7 @@
     <t>1982 - 2013</t>
   </si>
   <si>
-    <t>DIC faster</t>
-  </si>
-  <si>
-    <t>DIC fast</t>
+    <t>DIC</t>
   </si>
 </sst>
 </file>
@@ -89,7 +86,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +105,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -121,13 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,28 +421,26 @@
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="20" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F1" s="5" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F2" s="3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -449,66 +451,61 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
       <c r="G3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
         <v>94918.69</v>
       </c>
-      <c r="E4">
-        <v>94961.68</v>
+      <c r="F4" s="1">
+        <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="H4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5">
         <v>91192.639999999999</v>
       </c>
-      <c r="M4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <f>AVERAGE(D4,D6,D8,D10,D12,D14,D16,D18,D20,D22,I4,I6,I8,I10,I12,I14,I16,I18,I20,I22)</f>
+        <v>105828.51400000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -521,51 +518,53 @@
       <c r="D5">
         <v>94927.59</v>
       </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
       <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="H5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3">
         <v>91199.79</v>
       </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f>AVERAGE(D5,D7,D9,D11,D13,D15,D17,D19,D21,D23,I5,I7,I9,I11,I13,I15,I17,I19,I21,I23)</f>
+        <v>105821.71650000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3">
-        <v>76762.98</v>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>76711.929999999993</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
       </c>
       <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3">
         <v>71322.58</v>
       </c>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -578,22 +577,20 @@
       <c r="D7" s="3">
         <v>76724.14</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
       <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="5">
         <v>71327.509999999995</v>
       </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -606,52 +603,46 @@
       <c r="D8" s="3">
         <v>99378.62</v>
       </c>
-      <c r="E8" s="3">
-        <v>99423.16</v>
+      <c r="F8" s="1">
+        <v>2</v>
       </c>
       <c r="G8" s="1">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1">
         <v>15</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="H8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="6">
         <v>84903.43</v>
       </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5">
         <v>99374.81</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
       <c r="G9" s="1">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1">
         <v>15</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3">
         <v>84894.29</v>
       </c>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -664,54 +655,46 @@
       <c r="D10" s="3">
         <v>101188.67</v>
       </c>
-      <c r="E10" s="3">
-        <v>101230.06</v>
+      <c r="F10" s="2">
+        <v>2</v>
       </c>
       <c r="G10" s="2">
-        <v>2</v>
-      </c>
-      <c r="H10" s="2">
         <v>25</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="3">
+      <c r="H10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3">
         <v>89210.26</v>
       </c>
-      <c r="K10" s="3">
-        <v>89255.83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1</v>
       </c>
       <c r="B11" s="2">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5">
         <v>101178.52</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
       <c r="G11" s="2">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2">
         <v>25</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="3">
+      <c r="H11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="5">
         <v>89198.93</v>
       </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -724,54 +707,46 @@
       <c r="D12" s="3">
         <v>107571.26</v>
       </c>
-      <c r="E12" s="3">
-        <v>107609.46</v>
+      <c r="F12" s="1">
+        <v>2</v>
       </c>
       <c r="G12" s="1">
-        <v>2</v>
-      </c>
-      <c r="H12" s="1">
         <v>35</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="3">
+      <c r="H12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="5">
         <v>97878.080000000002</v>
       </c>
-      <c r="K12" s="3">
-        <v>97927.85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" s="1">
         <v>35</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5">
         <v>107563.33</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
       <c r="G13" s="1">
-        <v>2</v>
-      </c>
-      <c r="H13" s="1">
         <v>35</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="3">
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3">
         <v>97882.07</v>
       </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -784,86 +759,72 @@
       <c r="D14" s="3">
         <v>112656.62</v>
       </c>
-      <c r="E14" s="3">
-        <v>112695.3</v>
+      <c r="F14" s="2">
+        <v>2</v>
       </c>
       <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2">
         <v>45</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="3">
+      <c r="H14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="5">
         <v>104430.63</v>
       </c>
-      <c r="K14" s="3">
-        <v>104475.13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
       <c r="B15" s="2">
         <v>45</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5">
         <v>112653.75999999999</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
       <c r="G15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2">
         <v>45</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="3">
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3">
         <v>104433.18</v>
       </c>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
       </c>
       <c r="B16" s="1">
         <v>55</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
         <v>118127</v>
       </c>
-      <c r="E16" s="3">
-        <v>118142.8</v>
+      <c r="F16" s="1">
+        <v>2</v>
       </c>
       <c r="G16" s="1">
-        <v>2</v>
-      </c>
-      <c r="H16" s="1">
         <v>55</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="3">
+      <c r="H16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="5">
         <v>112259.12</v>
       </c>
-      <c r="K16" s="3">
-        <v>112278.31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -876,22 +837,20 @@
       <c r="D17" s="3">
         <v>118131.56</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
       <c r="G17" s="1">
-        <v>2</v>
-      </c>
-      <c r="H17" s="1">
         <v>55</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="3">
+      <c r="H17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="3">
         <v>112260.85</v>
       </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -904,54 +863,46 @@
       <c r="D18" s="3">
         <v>124111.61</v>
       </c>
-      <c r="E18" s="3">
-        <v>124116.03</v>
+      <c r="F18" s="2">
+        <v>2</v>
       </c>
       <c r="G18" s="2">
-        <v>2</v>
-      </c>
-      <c r="H18" s="2">
         <v>65</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J18" s="3">
+      <c r="H18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="5">
         <v>119666.94</v>
       </c>
-      <c r="K18" s="3">
-        <v>119686.86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>1</v>
       </c>
       <c r="B19" s="2">
         <v>65</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5">
         <v>124109.23</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
       <c r="G19" s="2">
-        <v>2</v>
-      </c>
-      <c r="H19" s="2">
         <v>65</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="3">
+      <c r="H19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="3">
         <v>119672.32000000001</v>
       </c>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -964,58 +915,46 @@
       <c r="D20" s="3">
         <v>126773.38</v>
       </c>
-      <c r="E20" s="3">
-        <v>126775.3</v>
+      <c r="F20" s="1">
+        <v>2</v>
       </c>
       <c r="G20" s="1">
-        <v>2</v>
-      </c>
-      <c r="H20" s="1">
         <v>75</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J20" s="3">
+      <c r="H20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3">
         <v>128179.43</v>
       </c>
-      <c r="K20" s="3">
-        <v>128194.93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21" s="1">
         <v>75</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="3">
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5">
         <v>126754.2</v>
       </c>
-      <c r="E21" s="3">
-        <v>126754.16</v>
+      <c r="F21" s="1">
+        <v>2</v>
       </c>
       <c r="G21" s="1">
-        <v>2</v>
-      </c>
-      <c r="H21" s="1">
         <v>75</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="H21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="5">
         <v>128142.2</v>
       </c>
-      <c r="K21" s="3">
-        <v>128142.16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1028,116 +967,94 @@
       <c r="D22" s="3">
         <v>122883.22</v>
       </c>
-      <c r="E22" s="3">
-        <v>122882.5</v>
+      <c r="F22" s="2">
+        <v>2</v>
       </c>
       <c r="G22" s="2">
-        <v>2</v>
-      </c>
-      <c r="H22" s="2">
         <v>85</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="3">
+      <c r="H22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="3">
         <v>133206.17000000001</v>
       </c>
-      <c r="K22" s="3">
-        <v>133227.74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>1</v>
       </c>
       <c r="B23" s="2">
         <v>85</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="C23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5">
         <v>122847.07</v>
       </c>
-      <c r="E23" s="3">
-        <v>122847.08</v>
+      <c r="F23" s="2">
+        <v>2</v>
       </c>
       <c r="G23" s="2">
-        <v>2</v>
-      </c>
-      <c r="H23" s="2">
         <v>85</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="3">
+      <c r="H23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="5">
         <v>133158.98000000001</v>
       </c>
-      <c r="K23" s="3">
-        <v>133158.97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>